<commit_message>
Control the TC Exec via flag
</commit_message>
<xml_diff>
--- a/src/test/resources/runmanager/TestExecution.xlsx
+++ b/src/test/resources/runmanager/TestExecution.xlsx
@@ -43,19 +43,19 @@
     <t xml:space="preserve">This test to Login and Logout Functionality</t>
   </si>
   <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing an another method</t>
+  </si>
+  <si>
     <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">newTest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testing an another method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
@@ -158,10 +158,10 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.99"/>
@@ -215,7 +215,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>12</v>

</xml_diff>